<commit_message>
Crawls the web and outputs top 5 links to websites about entity/topic
</commit_message>
<xml_diff>
--- a/ticker.xlsx
+++ b/ticker.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Apple Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">APPL</t>
+    <t xml:space="preserve">AAPL</t>
   </si>
   <si>
     <t xml:space="preserve">Tesla</t>
@@ -150,7 +150,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
add more companies to ticker.xlsx
</commit_message>
<xml_diff>
--- a/ticker.xlsx
+++ b/ticker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilycroxall/Documents/sentiment-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA8C4BC-C446-0540-8C76-FD29BAA3D414}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB44C4D1-1D0B-E041-8315-984978B0EE16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2140" yWindow="460" windowWidth="24400" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="674">
   <si>
     <t>Name</t>
   </si>
@@ -385,6 +385,1668 @@
   </si>
   <si>
     <t>AMT</t>
+  </si>
+  <si>
+    <t>General Electric Company</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>Altria Group Inc</t>
+  </si>
+  <si>
+    <t>Danaher Corporation</t>
+  </si>
+  <si>
+    <t>Lockheed Matrin Corporation</t>
+  </si>
+  <si>
+    <t>Gilead Sciences Inc.</t>
+  </si>
+  <si>
+    <t>American Express Company</t>
+  </si>
+  <si>
+    <t>Booking Holdings Inc.</t>
+  </si>
+  <si>
+    <t>Lowe's Companies Inc.</t>
+  </si>
+  <si>
+    <t>Mondelez International Inc. Class A</t>
+  </si>
+  <si>
+    <t>U.S. Bancorp</t>
+  </si>
+  <si>
+    <t>Caterpillar Inc.</t>
+  </si>
+  <si>
+    <t>Bristol-Myers Squibb Company</t>
+  </si>
+  <si>
+    <t>Anthem Inc.</t>
+  </si>
+  <si>
+    <t>CME Group Inc. Class A</t>
+  </si>
+  <si>
+    <t>United Parcel Service Inc. Class B</t>
+  </si>
+  <si>
+    <t>CVS Health Corporation</t>
+  </si>
+  <si>
+    <t>Automatic Data Processing Inc.</t>
+  </si>
+  <si>
+    <t>Goldman Sachs Group Inc.</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>DHR</t>
+  </si>
+  <si>
+    <t>LMT</t>
+  </si>
+  <si>
+    <t>GILD</t>
+  </si>
+  <si>
+    <t>AXP</t>
+  </si>
+  <si>
+    <t>BKNG</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>MDLZ</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>BMY</t>
+  </si>
+  <si>
+    <t>ANTM</t>
+  </si>
+  <si>
+    <t>CME</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>CVS</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>Intuit Inc.</t>
+  </si>
+  <si>
+    <t>Charter Communications Inc. Class A</t>
+  </si>
+  <si>
+    <t>Becton Dickinson and Company</t>
+  </si>
+  <si>
+    <t>Chubb Limited</t>
+  </si>
+  <si>
+    <t>ConocoPhillips</t>
+  </si>
+  <si>
+    <t>Celgene Corporation</t>
+  </si>
+  <si>
+    <t>Duke Energy Corporation</t>
+  </si>
+  <si>
+    <t>TJX Companies Inc</t>
+  </si>
+  <si>
+    <t>Stryker Corporation</t>
+  </si>
+  <si>
+    <t>PNC Financial Services Group Inc.</t>
+  </si>
+  <si>
+    <t>Colgate-Palmolive Company</t>
+  </si>
+  <si>
+    <t>Dominion Energy Inc.</t>
+  </si>
+  <si>
+    <t>Cigna Corporation</t>
+  </si>
+  <si>
+    <t>Intuitive Surgical Inc.</t>
+  </si>
+  <si>
+    <t>CSX Corporation</t>
+  </si>
+  <si>
+    <t>Boston Scientific Corporation</t>
+  </si>
+  <si>
+    <t>S&amp;P Gobal Inc.</t>
+  </si>
+  <si>
+    <t>Southern Company</t>
+  </si>
+  <si>
+    <t>BlackRock Inc.</t>
+  </si>
+  <si>
+    <t>Morgan Stanley</t>
+  </si>
+  <si>
+    <t>Crown Castle International Corp</t>
+  </si>
+  <si>
+    <t>DuPont de Nemours Inc.</t>
+  </si>
+  <si>
+    <t>Illumina Inc.</t>
+  </si>
+  <si>
+    <t>Northrop Grumman</t>
+  </si>
+  <si>
+    <t>INTU</t>
+  </si>
+  <si>
+    <t>CHTR</t>
+  </si>
+  <si>
+    <t>BDX</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>CELG</t>
+  </si>
+  <si>
+    <t>DUK</t>
+  </si>
+  <si>
+    <t>TJX</t>
+  </si>
+  <si>
+    <t>SYK</t>
+  </si>
+  <si>
+    <t>PNC</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>ISRG</t>
+  </si>
+  <si>
+    <t>CSX</t>
+  </si>
+  <si>
+    <t>BSX</t>
+  </si>
+  <si>
+    <t>SPGI</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>BLK</t>
+  </si>
+  <si>
+    <t>CCI</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>ILMN</t>
+  </si>
+  <si>
+    <t>NOC</t>
+  </si>
+  <si>
+    <t>Zoetis Inc. Class A</t>
+  </si>
+  <si>
+    <t>Schulmberger NV</t>
+  </si>
+  <si>
+    <t>Norfolk Southern Corporation</t>
+  </si>
+  <si>
+    <t>Marsh &amp; McLennan Companies Inc.</t>
+  </si>
+  <si>
+    <t>Allergan plc</t>
+  </si>
+  <si>
+    <t>Deere &amp; Company</t>
+  </si>
+  <si>
+    <t>Prologis Inc.</t>
+  </si>
+  <si>
+    <t>Air Products and Chemicals Inc.</t>
+  </si>
+  <si>
+    <t>Simon Property Group Inc.</t>
+  </si>
+  <si>
+    <t>Ecolab Inc.</t>
+  </si>
+  <si>
+    <t>EOG Resources Inc.</t>
+  </si>
+  <si>
+    <t>General Motors Company</t>
+  </si>
+  <si>
+    <t>Intercontinental Exchange Inc.</t>
+  </si>
+  <si>
+    <t>General Dynamics Corporations</t>
+  </si>
+  <si>
+    <t>Progressive Corporation</t>
+  </si>
+  <si>
+    <t>Raytheon Company</t>
+  </si>
+  <si>
+    <t>MetLife Inc.</t>
+  </si>
+  <si>
+    <t>Charles Schwab Corporation</t>
+  </si>
+  <si>
+    <t>American International Group Inc.</t>
+  </si>
+  <si>
+    <t>Aon plc</t>
+  </si>
+  <si>
+    <t>Exelon Corporation</t>
+  </si>
+  <si>
+    <t>Kimberly-Clark Corporation</t>
+  </si>
+  <si>
+    <t>Vertex Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>ZTS</t>
+  </si>
+  <si>
+    <t>SLB</t>
+  </si>
+  <si>
+    <t>NCS</t>
+  </si>
+  <si>
+    <t>MMC</t>
+  </si>
+  <si>
+    <t>AGN</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>PLD</t>
+  </si>
+  <si>
+    <t>APD</t>
+  </si>
+  <si>
+    <t>ECL</t>
+  </si>
+  <si>
+    <t>EOG</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>ICE</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>PGR</t>
+  </si>
+  <si>
+    <t>RTN</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>SCHW</t>
+  </si>
+  <si>
+    <t>AIG</t>
+  </si>
+  <si>
+    <t>AON</t>
+  </si>
+  <si>
+    <t>EXC</t>
+  </si>
+  <si>
+    <t>KMB</t>
+  </si>
+  <si>
+    <t>VRTX</t>
+  </si>
+  <si>
+    <t>Biogen Inc.</t>
+  </si>
+  <si>
+    <t>Waste Management Inc.</t>
+  </si>
+  <si>
+    <t>Illinois Tool Works Inc.</t>
+  </si>
+  <si>
+    <t>Target Corporation</t>
+  </si>
+  <si>
+    <t>American Electric Power Company Inc.</t>
+  </si>
+  <si>
+    <t>Micron Technology Inc.</t>
+  </si>
+  <si>
+    <t>Capital One Financial Corporation</t>
+  </si>
+  <si>
+    <t>Equinix Inc.</t>
+  </si>
+  <si>
+    <t>Walgreens Boots Alliance Inc</t>
+  </si>
+  <si>
+    <t>Aflac Incorporated</t>
+  </si>
+  <si>
+    <t>Applied Materials Inc.</t>
+  </si>
+  <si>
+    <t>Analog Devices Inc.</t>
+  </si>
+  <si>
+    <t>Prudential Financial Inc.</t>
+  </si>
+  <si>
+    <t>Fidelity National Information Services Inc.</t>
+  </si>
+  <si>
+    <t>Kinder Morgan Inc Class P</t>
+  </si>
+  <si>
+    <t>Emerson Electric Co.</t>
+  </si>
+  <si>
+    <t>Estee Lauder Companies Inc. Class A</t>
+  </si>
+  <si>
+    <t>Phillips 66</t>
+  </si>
+  <si>
+    <t>Travelers Companies Inc.</t>
+  </si>
+  <si>
+    <t>L3Harris Technologies Inc.</t>
+  </si>
+  <si>
+    <t>Ford Motor Company</t>
+  </si>
+  <si>
+    <t>BIIB</t>
+  </si>
+  <si>
+    <t>ITW</t>
+  </si>
+  <si>
+    <t>TGT</t>
+  </si>
+  <si>
+    <t>AEP</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>COF</t>
+  </si>
+  <si>
+    <t>EQIX</t>
+  </si>
+  <si>
+    <t>WBA</t>
+  </si>
+  <si>
+    <t>AFL</t>
+  </si>
+  <si>
+    <t>AMAT</t>
+  </si>
+  <si>
+    <t>ADI</t>
+  </si>
+  <si>
+    <t>PRU</t>
+  </si>
+  <si>
+    <t>FIS</t>
+  </si>
+  <si>
+    <t>KMI</t>
+  </si>
+  <si>
+    <t>EMR</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>PSX</t>
+  </si>
+  <si>
+    <t>TRV</t>
+  </si>
+  <si>
+    <t>LHX</t>
+  </si>
+  <si>
+    <t>BDK</t>
+  </si>
+  <si>
+    <t>Bank of New York Mellon Corporation</t>
+  </si>
+  <si>
+    <t>Marriott International Inc. Class A</t>
+  </si>
+  <si>
+    <t>Edwards Lifesciences Corporation</t>
+  </si>
+  <si>
+    <t>Roper Technologies Inc.</t>
+  </si>
+  <si>
+    <t>Baxter International Inc.</t>
+  </si>
+  <si>
+    <t>FedEx Corporation</t>
+  </si>
+  <si>
+    <t>Shermin-Williams Company</t>
+  </si>
+  <si>
+    <t>Autodesk Inc.</t>
+  </si>
+  <si>
+    <t>Sempra Energy</t>
+  </si>
+  <si>
+    <t>BB&amp;T Corporation</t>
+  </si>
+  <si>
+    <t>Activision Blizzard Inc.</t>
+  </si>
+  <si>
+    <t>Ross Stores Inc.</t>
+  </si>
+  <si>
+    <t>Public Storage</t>
+  </si>
+  <si>
+    <t>Dow Inc.</t>
+  </si>
+  <si>
+    <t>Cognizant Technology Solutions Corporation Class A</t>
+  </si>
+  <si>
+    <t>Fiserv Inc.</t>
+  </si>
+  <si>
+    <t>HCA Healthcare Inc</t>
+  </si>
+  <si>
+    <t>Occidental Petroleum Corporation</t>
+  </si>
+  <si>
+    <t>Marathon Petroleum Corporation</t>
+  </si>
+  <si>
+    <t>Dollar General Corporation</t>
+  </si>
+  <si>
+    <t>Anadarko Petroleum Corporation</t>
+  </si>
+  <si>
+    <t>Humana Inc.</t>
+  </si>
+  <si>
+    <t>Delta Air Lines Inc.</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>EW</t>
+  </si>
+  <si>
+    <t>ROP</t>
+  </si>
+  <si>
+    <t>BAX</t>
+  </si>
+  <si>
+    <t>FDX</t>
+  </si>
+  <si>
+    <t>SHW</t>
+  </si>
+  <si>
+    <t>ADSK</t>
+  </si>
+  <si>
+    <t>SRE</t>
+  </si>
+  <si>
+    <t>BBT</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
+    <t>ROST</t>
+  </si>
+  <si>
+    <t>PSA</t>
+  </si>
+  <si>
+    <t>DOW</t>
+  </si>
+  <si>
+    <t>CTSH</t>
+  </si>
+  <si>
+    <t>FISV</t>
+  </si>
+  <si>
+    <t>HCA</t>
+  </si>
+  <si>
+    <t>OXY</t>
+  </si>
+  <si>
+    <t>MPC</t>
+  </si>
+  <si>
+    <t>DG</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>HUM</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>Eaton Corp. Plc</t>
+  </si>
+  <si>
+    <t>Allstate Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wellstower Inc. </t>
+  </si>
+  <si>
+    <t>Valero Energy Corporation</t>
+  </si>
+  <si>
+    <t>Yum! Brands Inc.</t>
+  </si>
+  <si>
+    <t>Sysco Corporation</t>
+  </si>
+  <si>
+    <t>Moody's Corporation</t>
+  </si>
+  <si>
+    <t>Red Hat Inc.</t>
+  </si>
+  <si>
+    <t>Johnson Controls International plc</t>
+  </si>
+  <si>
+    <t>Constellation Brands Inc. Class A</t>
+  </si>
+  <si>
+    <t>eBay Inc.</t>
+  </si>
+  <si>
+    <t>TE Connectivity Ltd.</t>
+  </si>
+  <si>
+    <t>HP Inc.</t>
+  </si>
+  <si>
+    <t>General Mills Inc.</t>
+  </si>
+  <si>
+    <t>Newmont Goldcorp Corporation</t>
+  </si>
+  <si>
+    <t>Xcel Energy Inc.</t>
+  </si>
+  <si>
+    <t>O'Reilly Automotive Inc.</t>
+  </si>
+  <si>
+    <t>Ingersoll-Rand Plc</t>
+  </si>
+  <si>
+    <t>Public Service Enterprise Group Inc</t>
+  </si>
+  <si>
+    <t>Alexion Pharmaceuticals Inc.</t>
+  </si>
+  <si>
+    <t>Amphenol Corporation Class A</t>
+  </si>
+  <si>
+    <t>ETN</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>WELL</t>
+  </si>
+  <si>
+    <t>VLO</t>
+  </si>
+  <si>
+    <t>WMB</t>
+  </si>
+  <si>
+    <t>YUM</t>
+  </si>
+  <si>
+    <t>SYY</t>
+  </si>
+  <si>
+    <t>MCO</t>
+  </si>
+  <si>
+    <t>RHT</t>
+  </si>
+  <si>
+    <t>JCI</t>
+  </si>
+  <si>
+    <t>STZ</t>
+  </si>
+  <si>
+    <t>EBAY</t>
+  </si>
+  <si>
+    <t>TEL</t>
+  </si>
+  <si>
+    <t>HPQ</t>
+  </si>
+  <si>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEM </t>
+  </si>
+  <si>
+    <t>XEL</t>
+  </si>
+  <si>
+    <t>ORLY</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>PEG</t>
+  </si>
+  <si>
+    <t>ALXN</t>
+  </si>
+  <si>
+    <t>Williams Companies Inc.</t>
+  </si>
+  <si>
+    <t>APH</t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>Hilton Worldwide Holdings Inc.</t>
+  </si>
+  <si>
+    <t>Electronic Arts Inc.</t>
+  </si>
+  <si>
+    <t>Xilinx Inc.</t>
+  </si>
+  <si>
+    <t>Consolidated Edison Inc.</t>
+  </si>
+  <si>
+    <t>AvalonBay Communities Inc.</t>
+  </si>
+  <si>
+    <t>Equity Residential</t>
+  </si>
+  <si>
+    <t>ONEOK Inc.</t>
+  </si>
+  <si>
+    <t>V.F. Corporation</t>
+  </si>
+  <si>
+    <t>PPG Industries Inc.</t>
+  </si>
+  <si>
+    <t>Motorola Solutions Inc.</t>
+  </si>
+  <si>
+    <t>Lam Research Corporation</t>
+  </si>
+  <si>
+    <t>AutoZone Inc.</t>
+  </si>
+  <si>
+    <t>SunTrust Banks Inc.</t>
+  </si>
+  <si>
+    <t>Advanced Micro Devices Inc.</t>
+  </si>
+  <si>
+    <t>Paychex Inc.</t>
+  </si>
+  <si>
+    <t>McKesson Corporation</t>
+  </si>
+  <si>
+    <t>WEC Energy Group Inc.</t>
+  </si>
+  <si>
+    <t>LyondellBasell Industries NV</t>
+  </si>
+  <si>
+    <t>SBA Communications Corp. Class A</t>
+  </si>
+  <si>
+    <t>Corning Inc.</t>
+  </si>
+  <si>
+    <t>Discover Financial Services</t>
+  </si>
+  <si>
+    <t>T. Rowe Price Group</t>
+  </si>
+  <si>
+    <t>Twitter Inc.</t>
+  </si>
+  <si>
+    <t>Ventas Inc.</t>
+  </si>
+  <si>
+    <t>Dollar Tree Inc.</t>
+  </si>
+  <si>
+    <t>Monster Beverage Corporation</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>XLNX</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>AVB</t>
+  </si>
+  <si>
+    <t>EQR</t>
+  </si>
+  <si>
+    <t>OKE</t>
+  </si>
+  <si>
+    <t>VFC</t>
+  </si>
+  <si>
+    <t>PPG</t>
+  </si>
+  <si>
+    <t>MSI</t>
+  </si>
+  <si>
+    <t>LRCX</t>
+  </si>
+  <si>
+    <t>AZO</t>
+  </si>
+  <si>
+    <t>STI</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>PAYX</t>
+  </si>
+  <si>
+    <t>MCK</t>
+  </si>
+  <si>
+    <t>WEC</t>
+  </si>
+  <si>
+    <t>LYB</t>
+  </si>
+  <si>
+    <t>SBAC</t>
+  </si>
+  <si>
+    <t>SLW</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>TROW</t>
+  </si>
+  <si>
+    <t>TWTR</t>
+  </si>
+  <si>
+    <t>VTR</t>
+  </si>
+  <si>
+    <t>DLTR</t>
+  </si>
+  <si>
+    <t>MNST</t>
+  </si>
+  <si>
+    <t>Southwest Airlines Co.</t>
+  </si>
+  <si>
+    <t>IQVIA Holdings Inc.</t>
+  </si>
+  <si>
+    <t>Global Payments Inc.</t>
+  </si>
+  <si>
+    <t>Willis Towers Watson Public Limited Company</t>
+  </si>
+  <si>
+    <t>FleetCor Technologies Inc.</t>
+  </si>
+  <si>
+    <t>Digital Realty Trust Inc.</t>
+  </si>
+  <si>
+    <t>Regeneron Pharmaceuticals Inc.</t>
+  </si>
+  <si>
+    <t>Eversource Energy</t>
+  </si>
+  <si>
+    <t>Ball Corporation</t>
+  </si>
+  <si>
+    <t>PACCAR Inc.</t>
+  </si>
+  <si>
+    <t>Cummins Inc.</t>
+  </si>
+  <si>
+    <t>Verisk Analystics Inc</t>
+  </si>
+  <si>
+    <t>Fortive Corp</t>
+  </si>
+  <si>
+    <t>Pioneer Natural Resources Company</t>
+  </si>
+  <si>
+    <t>Agilent Technologies Inc.</t>
+  </si>
+  <si>
+    <t>Tyson Foods Inc. Class A</t>
+  </si>
+  <si>
+    <t>Cerner Corporation</t>
+  </si>
+  <si>
+    <t>TransDigm Group Incorporatied</t>
+  </si>
+  <si>
+    <t>Zimmer Biomet Holdings Inc.</t>
+  </si>
+  <si>
+    <t>DTE Energy Company</t>
+  </si>
+  <si>
+    <t>IDEXX Laboratories Inc.</t>
+  </si>
+  <si>
+    <t>M&amp;T Bank Corporation</t>
+  </si>
+  <si>
+    <t>IHS Markit Ltd.</t>
+  </si>
+  <si>
+    <t>Archer-Daniels-Midland Company</t>
+  </si>
+  <si>
+    <t>LUV</t>
+  </si>
+  <si>
+    <t>IQV</t>
+  </si>
+  <si>
+    <t>GPN</t>
+  </si>
+  <si>
+    <t>WLTW</t>
+  </si>
+  <si>
+    <t>FLT</t>
+  </si>
+  <si>
+    <t>DLR</t>
+  </si>
+  <si>
+    <t>REGN</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>BLL</t>
+  </si>
+  <si>
+    <t>PCAR</t>
+  </si>
+  <si>
+    <t>CMI</t>
+  </si>
+  <si>
+    <t>CRSK</t>
+  </si>
+  <si>
+    <t>FTV</t>
+  </si>
+  <si>
+    <t>PXD</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>TSN</t>
+  </si>
+  <si>
+    <t>CERN</t>
+  </si>
+  <si>
+    <t>TDG</t>
+  </si>
+  <si>
+    <t>ZBH</t>
+  </si>
+  <si>
+    <t>DTE</t>
+  </si>
+  <si>
+    <t>IDXX</t>
+  </si>
+  <si>
+    <t>MTB</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>VeriSign Inc.</t>
+  </si>
+  <si>
+    <t>Synchrony Financial</t>
+  </si>
+  <si>
+    <t>PPL Corporation</t>
+  </si>
+  <si>
+    <t>Realty Income Corporation</t>
+  </si>
+  <si>
+    <t>Stanley Black &amp; Decker Inc.</t>
+  </si>
+  <si>
+    <t>FirstEnergy Corp.</t>
+  </si>
+  <si>
+    <t>Edison International</t>
+  </si>
+  <si>
+    <t>Parker-Hannifin Corporation</t>
+  </si>
+  <si>
+    <t>Total System Services Inc.</t>
+  </si>
+  <si>
+    <t>Mettler-Toledo International Inc.</t>
+  </si>
+  <si>
+    <t>Corteva Inc</t>
+  </si>
+  <si>
+    <t>American Water Works Company Inc.</t>
+  </si>
+  <si>
+    <t>Microchip Technology Incorporated</t>
+  </si>
+  <si>
+    <t>State Street Corporation</t>
+  </si>
+  <si>
+    <t>Centene Corporation</t>
+  </si>
+  <si>
+    <t>Cadence Design Systems Inc</t>
+  </si>
+  <si>
+    <t>AMETEK Inc.</t>
+  </si>
+  <si>
+    <t>Aptiv PLC</t>
+  </si>
+  <si>
+    <t>MSCI Inc. Class A</t>
+  </si>
+  <si>
+    <t>Hewlett Packard Enterprise Co.</t>
+  </si>
+  <si>
+    <t>Boston Properties Inc.</t>
+  </si>
+  <si>
+    <t>Hartford Financial Services Group Inc.</t>
+  </si>
+  <si>
+    <t>Fifth Third Bancorp</t>
+  </si>
+  <si>
+    <t>VRSN</t>
+  </si>
+  <si>
+    <t>SYF</t>
+  </si>
+  <si>
+    <t>PPL</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>SWK</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>EIX</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>TSS</t>
+  </si>
+  <si>
+    <t>MTD</t>
+  </si>
+  <si>
+    <t>CTVA</t>
+  </si>
+  <si>
+    <t>AWK</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>MCHP</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>CDNS</t>
+  </si>
+  <si>
+    <t>AME</t>
+  </si>
+  <si>
+    <t>APTV</t>
+  </si>
+  <si>
+    <t>MSCI</t>
+  </si>
+  <si>
+    <t>HPE</t>
+  </si>
+  <si>
+    <t>BXP</t>
+  </si>
+  <si>
+    <t>HIG</t>
+  </si>
+  <si>
+    <t>FITB</t>
+  </si>
+  <si>
+    <t>United Airlines Holdings Inc</t>
+  </si>
+  <si>
+    <t>Northern Trust Corporation</t>
+  </si>
+  <si>
+    <t>Cintas Corporation</t>
+  </si>
+  <si>
+    <t>Synopsys Inc</t>
+  </si>
+  <si>
+    <t>Clorox Company</t>
+  </si>
+  <si>
+    <t>Ameriprise Financial Inc</t>
+  </si>
+  <si>
+    <t>Royal Caribbean Cruises Ltd.</t>
+  </si>
+  <si>
+    <t>Weyerhaeuser Compay</t>
+  </si>
+  <si>
+    <t>McCormick &amp; Company Incorporated</t>
+  </si>
+  <si>
+    <t>Align Technology Inc.</t>
+  </si>
+  <si>
+    <t>Halliburton Company</t>
+  </si>
+  <si>
+    <t>Essex Property Trust Inc.</t>
+  </si>
+  <si>
+    <t>Concho Resources Inc.</t>
+  </si>
+  <si>
+    <t>Entergy Corporation</t>
+  </si>
+  <si>
+    <t>KLA-Tencor Corporation</t>
+  </si>
+  <si>
+    <t>Rockwell Automation Inc.</t>
+  </si>
+  <si>
+    <t>Kraft Heinz Company</t>
+  </si>
+  <si>
+    <t>Ulta Beauty Inc.</t>
+  </si>
+  <si>
+    <t>Hershey Company</t>
+  </si>
+  <si>
+    <t>Amcor PLC</t>
+  </si>
+  <si>
+    <t>Republic Services Inc.</t>
+  </si>
+  <si>
+    <t>Omnicom Group Inc.</t>
+  </si>
+  <si>
+    <t>Ameren Corporation</t>
+  </si>
+  <si>
+    <t>Vulcan Materials Company</t>
+  </si>
+  <si>
+    <t>Fastenal Company</t>
+  </si>
+  <si>
+    <t>UAL</t>
+  </si>
+  <si>
+    <t>NTRS</t>
+  </si>
+  <si>
+    <t>CTAS</t>
+  </si>
+  <si>
+    <t>SNPS</t>
+  </si>
+  <si>
+    <t>CLX</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>RCL</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>MKC</t>
+  </si>
+  <si>
+    <t>ALGN</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>CXO</t>
+  </si>
+  <si>
+    <t>ETR</t>
+  </si>
+  <si>
+    <t>KLAC</t>
+  </si>
+  <si>
+    <t>ROK</t>
+  </si>
+  <si>
+    <t>KHC</t>
+  </si>
+  <si>
+    <t>ULTA</t>
+  </si>
+  <si>
+    <t>HSY</t>
+  </si>
+  <si>
+    <t>AMCR</t>
+  </si>
+  <si>
+    <t>RSG</t>
+  </si>
+  <si>
+    <t>OMC</t>
+  </si>
+  <si>
+    <t>AEE</t>
+  </si>
+  <si>
+    <t>VMC</t>
+  </si>
+  <si>
+    <t>FAST</t>
+  </si>
+  <si>
+    <t>Church &amp; Dwight Co. Inc.</t>
+  </si>
+  <si>
+    <t>Carnival Corporation</t>
+  </si>
+  <si>
+    <t>CBS Corporation Class B</t>
+  </si>
+  <si>
+    <t>KeyCorp</t>
+  </si>
+  <si>
+    <t>International Paper Company</t>
+  </si>
+  <si>
+    <t>Chipotle Mexican Grill Inc.</t>
+  </si>
+  <si>
+    <t>ResMed Inc.</t>
+  </si>
+  <si>
+    <t>Laboratory Corporation of America Holdings</t>
+  </si>
+  <si>
+    <t>ANSYS Inc.</t>
+  </si>
+  <si>
+    <t>Kroger Co.</t>
+  </si>
+  <si>
+    <t>Nucor Corporation</t>
+  </si>
+  <si>
+    <t>Keysight Technologies Inc</t>
+  </si>
+  <si>
+    <t>maxim Integrated Products Inc.</t>
+  </si>
+  <si>
+    <t>Arthur J. Gallagher &amp; Co.</t>
+  </si>
+  <si>
+    <t>CMS Energy Corporation</t>
+  </si>
+  <si>
+    <t>Best Buy Co. Inc.</t>
+  </si>
+  <si>
+    <t>Equifax Inc.</t>
+  </si>
+  <si>
+    <t>Citizens Financial Group Inc.</t>
+  </si>
+  <si>
+    <t>First Republic Bank</t>
+  </si>
+  <si>
+    <t>CBRE Group Inc. Class A</t>
+  </si>
+  <si>
+    <t>Cooper Companies Inc.</t>
+  </si>
+  <si>
+    <t>Alexandria Real Estate Equities Inc.</t>
+  </si>
+  <si>
+    <t>Cincinnati Financial Corporation</t>
+  </si>
+  <si>
+    <t>Diamondback Energy Inc.</t>
+  </si>
+  <si>
+    <t>CHD</t>
+  </si>
+  <si>
+    <t>CCL</t>
+  </si>
+  <si>
+    <t>CBS</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>CMG</t>
+  </si>
+  <si>
+    <t>RMD</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <t>ANSS</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>NUE</t>
+  </si>
+  <si>
+    <t>KEYS</t>
+  </si>
+  <si>
+    <t>MXIM</t>
+  </si>
+  <si>
+    <t>AJG</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>BBY</t>
+  </si>
+  <si>
+    <t>EFX</t>
+  </si>
+  <si>
+    <t>CFG</t>
+  </si>
+  <si>
+    <t>FRC</t>
+  </si>
+  <si>
+    <t>CBRE</t>
+  </si>
+  <si>
+    <t>COO</t>
+  </si>
+  <si>
+    <t>ARE</t>
+  </si>
+  <si>
+    <t>CINF</t>
+  </si>
+  <si>
+    <t>FANG</t>
+  </si>
+  <si>
+    <t>Freeport-McMoRan Inc.</t>
+  </si>
+  <si>
+    <t>Symantec Corporation</t>
+  </si>
+  <si>
+    <t>Hess Corporation</t>
+  </si>
+  <si>
+    <t>Waters Corporation</t>
+  </si>
+  <si>
+    <t>Expedia Group inc.</t>
+  </si>
+  <si>
+    <t>HCP Inc.</t>
+  </si>
+  <si>
+    <t>Genuine Parts Company</t>
+  </si>
+  <si>
+    <t>Regions Financial Corporation</t>
+  </si>
+  <si>
+    <t>Teleflex Incorporated</t>
+  </si>
+  <si>
+    <t>Loews Corporation</t>
+  </si>
+  <si>
+    <t>NetApp Inc.</t>
+  </si>
+  <si>
+    <t>Incyte Corporation</t>
+  </si>
+  <si>
+    <t>Principal Financial Group Inc.</t>
+  </si>
+  <si>
+    <t>Broadridge Financial Solutions Inc</t>
+  </si>
+  <si>
+    <t>Dover Corporation</t>
+  </si>
+  <si>
+    <t>Evergy Inc.</t>
+  </si>
+  <si>
+    <t>Gartner Inc.</t>
+  </si>
+  <si>
+    <t>Xylem Inc.</t>
+  </si>
+  <si>
+    <t>D.R. Horton Inc.</t>
+  </si>
+  <si>
+    <t>Copart Inc.</t>
+  </si>
+  <si>
+    <t>DXC Technology Co.</t>
+  </si>
+  <si>
+    <t>Darden Restaurants Inc.</t>
+  </si>
+  <si>
+    <t>CarMax Inc.</t>
+  </si>
+  <si>
+    <t>CenterPoint Energy Inc.</t>
+  </si>
+  <si>
+    <t>MGM Resorts International</t>
+  </si>
+  <si>
+    <t>Huntington Bancshares Incorporated</t>
+  </si>
+  <si>
+    <t>FCX</t>
+  </si>
+  <si>
+    <t>SYMC</t>
+  </si>
+  <si>
+    <t>HES</t>
+  </si>
+  <si>
+    <t>WAT</t>
+  </si>
+  <si>
+    <t>EXPE</t>
+  </si>
+  <si>
+    <t>HCP</t>
+  </si>
+  <si>
+    <t>GPC</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>TFX</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>NTAP</t>
+  </si>
+  <si>
+    <t>INCY</t>
+  </si>
+  <si>
+    <t>PFG</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>DOV</t>
+  </si>
+  <si>
+    <t>EVRG</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>XYL</t>
+  </si>
+  <si>
+    <t>DHI</t>
+  </si>
+  <si>
+    <t>CPRT</t>
+  </si>
+  <si>
+    <t>DXC</t>
+  </si>
+  <si>
+    <t>DRI</t>
+  </si>
+  <si>
+    <t>KMX</t>
+  </si>
+  <si>
+    <t>CNP</t>
+  </si>
+  <si>
+    <t>MGM</t>
+  </si>
+  <si>
+    <t>HBAN</t>
   </si>
 </sst>
 </file>
@@ -736,10 +2398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A308" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B340" sqref="B340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1228,6 +2890,2238 @@
         <v>119</v>
       </c>
     </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>131</v>
+      </c>
+      <c r="B71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>135</v>
+      </c>
+      <c r="B75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>165</v>
+      </c>
+      <c r="B88" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>169</v>
+      </c>
+      <c r="B92" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>173</v>
+      </c>
+      <c r="B96" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>176</v>
+      </c>
+      <c r="B99" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>203</v>
+      </c>
+      <c r="B103" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>206</v>
+      </c>
+      <c r="B106" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>207</v>
+      </c>
+      <c r="B107" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>208</v>
+      </c>
+      <c r="B108" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>210</v>
+      </c>
+      <c r="B110" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>211</v>
+      </c>
+      <c r="B111" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>212</v>
+      </c>
+      <c r="B112" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>213</v>
+      </c>
+      <c r="B113" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>214</v>
+      </c>
+      <c r="B114" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>215</v>
+      </c>
+      <c r="B115" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>216</v>
+      </c>
+      <c r="B116" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>217</v>
+      </c>
+      <c r="B117" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>218</v>
+      </c>
+      <c r="B118" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>219</v>
+      </c>
+      <c r="B119" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>220</v>
+      </c>
+      <c r="B120" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>221</v>
+      </c>
+      <c r="B121" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>222</v>
+      </c>
+      <c r="B122" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>223</v>
+      </c>
+      <c r="B123" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>224</v>
+      </c>
+      <c r="B124" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>225</v>
+      </c>
+      <c r="B125" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>249</v>
+      </c>
+      <c r="B127" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>250</v>
+      </c>
+      <c r="B128" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>251</v>
+      </c>
+      <c r="B129" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>252</v>
+      </c>
+      <c r="B130" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>253</v>
+      </c>
+      <c r="B131" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>254</v>
+      </c>
+      <c r="B132" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>255</v>
+      </c>
+      <c r="B133" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>256</v>
+      </c>
+      <c r="B134" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>257</v>
+      </c>
+      <c r="B135" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>258</v>
+      </c>
+      <c r="B136" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>259</v>
+      </c>
+      <c r="B137" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>260</v>
+      </c>
+      <c r="B138" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>261</v>
+      </c>
+      <c r="B139" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>262</v>
+      </c>
+      <c r="B140" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>263</v>
+      </c>
+      <c r="B141" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>264</v>
+      </c>
+      <c r="B142" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>265</v>
+      </c>
+      <c r="B143" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>266</v>
+      </c>
+      <c r="B144" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>267</v>
+      </c>
+      <c r="B145" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>268</v>
+      </c>
+      <c r="B146" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>289</v>
+      </c>
+      <c r="B147" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>290</v>
+      </c>
+      <c r="B148" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>291</v>
+      </c>
+      <c r="B149" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>292</v>
+      </c>
+      <c r="B150" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>293</v>
+      </c>
+      <c r="B151" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>294</v>
+      </c>
+      <c r="B152" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>295</v>
+      </c>
+      <c r="B153" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>296</v>
+      </c>
+      <c r="B154" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>297</v>
+      </c>
+      <c r="B155" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>298</v>
+      </c>
+      <c r="B156" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>299</v>
+      </c>
+      <c r="B157" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>300</v>
+      </c>
+      <c r="B158" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>301</v>
+      </c>
+      <c r="B159" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>302</v>
+      </c>
+      <c r="B160" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>303</v>
+      </c>
+      <c r="B161" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>304</v>
+      </c>
+      <c r="B162" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>305</v>
+      </c>
+      <c r="B163" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>306</v>
+      </c>
+      <c r="B164" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>307</v>
+      </c>
+      <c r="B165" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>308</v>
+      </c>
+      <c r="B166" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>309</v>
+      </c>
+      <c r="B167" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>310</v>
+      </c>
+      <c r="B168" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>311</v>
+      </c>
+      <c r="B169" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>334</v>
+      </c>
+      <c r="B170" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>335</v>
+      </c>
+      <c r="B171" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>336</v>
+      </c>
+      <c r="B172" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>337</v>
+      </c>
+      <c r="B173" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>376</v>
+      </c>
+      <c r="B174" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>338</v>
+      </c>
+      <c r="B175" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>339</v>
+      </c>
+      <c r="B176" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>340</v>
+      </c>
+      <c r="B177" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>341</v>
+      </c>
+      <c r="B178" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>342</v>
+      </c>
+      <c r="B179" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>343</v>
+      </c>
+      <c r="B180" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>344</v>
+      </c>
+      <c r="B181" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>345</v>
+      </c>
+      <c r="B182" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>346</v>
+      </c>
+      <c r="B183" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>347</v>
+      </c>
+      <c r="B184" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>348</v>
+      </c>
+      <c r="B185" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>349</v>
+      </c>
+      <c r="B186" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>350</v>
+      </c>
+      <c r="B187" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>351</v>
+      </c>
+      <c r="B188" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>352</v>
+      </c>
+      <c r="B189" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>353</v>
+      </c>
+      <c r="B190" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>354</v>
+      </c>
+      <c r="B191" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>379</v>
+      </c>
+      <c r="B192" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>380</v>
+      </c>
+      <c r="B193" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>381</v>
+      </c>
+      <c r="B194" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>382</v>
+      </c>
+      <c r="B195" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>383</v>
+      </c>
+      <c r="B196" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>384</v>
+      </c>
+      <c r="B197" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>385</v>
+      </c>
+      <c r="B198" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>386</v>
+      </c>
+      <c r="B199" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>387</v>
+      </c>
+      <c r="B200" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>388</v>
+      </c>
+      <c r="B201" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>389</v>
+      </c>
+      <c r="B202" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>390</v>
+      </c>
+      <c r="B203" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>391</v>
+      </c>
+      <c r="B204" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>392</v>
+      </c>
+      <c r="B205" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>393</v>
+      </c>
+      <c r="B206" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>394</v>
+      </c>
+      <c r="B207" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>395</v>
+      </c>
+      <c r="B208" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>396</v>
+      </c>
+      <c r="B209" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>397</v>
+      </c>
+      <c r="B210" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>398</v>
+      </c>
+      <c r="B211" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>399</v>
+      </c>
+      <c r="B212" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>400</v>
+      </c>
+      <c r="B213" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>401</v>
+      </c>
+      <c r="B214" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>402</v>
+      </c>
+      <c r="B215" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>403</v>
+      </c>
+      <c r="B216" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>404</v>
+      </c>
+      <c r="B217" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>430</v>
+      </c>
+      <c r="B218" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>431</v>
+      </c>
+      <c r="B219" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>432</v>
+      </c>
+      <c r="B220" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>433</v>
+      </c>
+      <c r="B221" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>434</v>
+      </c>
+      <c r="B222" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>435</v>
+      </c>
+      <c r="B223" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>436</v>
+      </c>
+      <c r="B224" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>437</v>
+      </c>
+      <c r="B225" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>438</v>
+      </c>
+      <c r="B226" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>439</v>
+      </c>
+      <c r="B227" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>440</v>
+      </c>
+      <c r="B228" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>441</v>
+      </c>
+      <c r="B229" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>442</v>
+      </c>
+      <c r="B230" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>443</v>
+      </c>
+      <c r="B231" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>444</v>
+      </c>
+      <c r="B232" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>445</v>
+      </c>
+      <c r="B233" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>446</v>
+      </c>
+      <c r="B234" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>447</v>
+      </c>
+      <c r="B235" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>448</v>
+      </c>
+      <c r="B236" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>449</v>
+      </c>
+      <c r="B237" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>450</v>
+      </c>
+      <c r="B238" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>451</v>
+      </c>
+      <c r="B239" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>452</v>
+      </c>
+      <c r="B240" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>453</v>
+      </c>
+      <c r="B241" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>478</v>
+      </c>
+      <c r="B242" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>479</v>
+      </c>
+      <c r="B243" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>480</v>
+      </c>
+      <c r="B244" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>481</v>
+      </c>
+      <c r="B245" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>482</v>
+      </c>
+      <c r="B246" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>483</v>
+      </c>
+      <c r="B247" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>484</v>
+      </c>
+      <c r="B248" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>485</v>
+      </c>
+      <c r="B249" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>486</v>
+      </c>
+      <c r="B250" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>487</v>
+      </c>
+      <c r="B251" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>488</v>
+      </c>
+      <c r="B252" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>489</v>
+      </c>
+      <c r="B253" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>491</v>
+      </c>
+      <c r="B254" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>490</v>
+      </c>
+      <c r="B255" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>492</v>
+      </c>
+      <c r="B256" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>493</v>
+      </c>
+      <c r="B257" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>494</v>
+      </c>
+      <c r="B258" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>495</v>
+      </c>
+      <c r="B259" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>496</v>
+      </c>
+      <c r="B260" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>497</v>
+      </c>
+      <c r="B261" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>498</v>
+      </c>
+      <c r="B262" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>499</v>
+      </c>
+      <c r="B263" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>500</v>
+      </c>
+      <c r="B264" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>524</v>
+      </c>
+      <c r="B265" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>525</v>
+      </c>
+      <c r="B266" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>526</v>
+      </c>
+      <c r="B267" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>527</v>
+      </c>
+      <c r="B268" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>528</v>
+      </c>
+      <c r="B269" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>529</v>
+      </c>
+      <c r="B270" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>530</v>
+      </c>
+      <c r="B271" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>531</v>
+      </c>
+      <c r="B272" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>532</v>
+      </c>
+      <c r="B273" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>533</v>
+      </c>
+      <c r="B274" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>534</v>
+      </c>
+      <c r="B275" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>535</v>
+      </c>
+      <c r="B276" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>536</v>
+      </c>
+      <c r="B277" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>537</v>
+      </c>
+      <c r="B278" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>538</v>
+      </c>
+      <c r="B279" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>539</v>
+      </c>
+      <c r="B280" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>540</v>
+      </c>
+      <c r="B281" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>541</v>
+      </c>
+      <c r="B282" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>542</v>
+      </c>
+      <c r="B283" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>543</v>
+      </c>
+      <c r="B284" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>544</v>
+      </c>
+      <c r="B285" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>545</v>
+      </c>
+      <c r="B286" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>546</v>
+      </c>
+      <c r="B287" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>547</v>
+      </c>
+      <c r="B288" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>548</v>
+      </c>
+      <c r="B289" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>574</v>
+      </c>
+      <c r="B290" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>575</v>
+      </c>
+      <c r="B291" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>576</v>
+      </c>
+      <c r="B292" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>577</v>
+      </c>
+      <c r="B293" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>578</v>
+      </c>
+      <c r="B294" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>579</v>
+      </c>
+      <c r="B295" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>580</v>
+      </c>
+      <c r="B296" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>581</v>
+      </c>
+      <c r="B297" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>582</v>
+      </c>
+      <c r="B298" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>583</v>
+      </c>
+      <c r="B299" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>584</v>
+      </c>
+      <c r="B300" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>585</v>
+      </c>
+      <c r="B301" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>586</v>
+      </c>
+      <c r="B302" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>587</v>
+      </c>
+      <c r="B303" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>588</v>
+      </c>
+      <c r="B304" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>589</v>
+      </c>
+      <c r="B305" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>590</v>
+      </c>
+      <c r="B306" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
+        <v>591</v>
+      </c>
+      <c r="B307" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>592</v>
+      </c>
+      <c r="B308" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>593</v>
+      </c>
+      <c r="B309" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>594</v>
+      </c>
+      <c r="B310" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>595</v>
+      </c>
+      <c r="B311" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>596</v>
+      </c>
+      <c r="B312" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>597</v>
+      </c>
+      <c r="B313" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>622</v>
+      </c>
+      <c r="B314" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>623</v>
+      </c>
+      <c r="B315" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>624</v>
+      </c>
+      <c r="B316" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>625</v>
+      </c>
+      <c r="B317" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>626</v>
+      </c>
+      <c r="B318" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>627</v>
+      </c>
+      <c r="B319" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>628</v>
+      </c>
+      <c r="B320" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>629</v>
+      </c>
+      <c r="B321" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>630</v>
+      </c>
+      <c r="B322" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>631</v>
+      </c>
+      <c r="B323" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>632</v>
+      </c>
+      <c r="B324" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>633</v>
+      </c>
+      <c r="B325" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>634</v>
+      </c>
+      <c r="B326" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>635</v>
+      </c>
+      <c r="B327" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" t="s">
+        <v>636</v>
+      </c>
+      <c r="B328" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>637</v>
+      </c>
+      <c r="B329" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>638</v>
+      </c>
+      <c r="B330" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>639</v>
+      </c>
+      <c r="B331" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>640</v>
+      </c>
+      <c r="B332" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>641</v>
+      </c>
+      <c r="B333" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>642</v>
+      </c>
+      <c r="B334" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>643</v>
+      </c>
+      <c r="B335" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>644</v>
+      </c>
+      <c r="B336" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>645</v>
+      </c>
+      <c r="B337" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>646</v>
+      </c>
+      <c r="B338" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>647</v>
+      </c>
+      <c r="B339" t="s">
+        <v>673</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
adds some changes somewhere I think
</commit_message>
<xml_diff>
--- a/ticker.xlsx
+++ b/ticker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilycroxall/Documents/sentiment-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB44C4D1-1D0B-E041-8315-984978B0EE16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73C1D73-97F5-F046-B329-77F8B2889DBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="460" windowWidth="24400" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Apple Inc</t>
   </si>
   <si>
-    <t>Tesla</t>
-  </si>
-  <si>
     <t>TSLA</t>
   </si>
   <si>
@@ -2047,6 +2044,9 @@
   </si>
   <si>
     <t>HBAN</t>
+  </si>
+  <si>
+    <t>Tesla, Inc.</t>
   </si>
 </sst>
 </file>
@@ -2400,8 +2400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A308" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B340" sqref="B340"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2423,2703 +2423,2703 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>673</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
         <v>60</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
         <v>62</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
         <v>64</v>
-      </c>
-      <c r="B33" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
         <v>66</v>
-      </c>
-      <c r="B34" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
         <v>68</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
         <v>70</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
         <v>72</v>
-      </c>
-      <c r="B37" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
         <v>74</v>
-      </c>
-      <c r="B38" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
         <v>76</v>
-      </c>
-      <c r="B39" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
         <v>78</v>
-      </c>
-      <c r="B40" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
         <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" t="s">
         <v>82</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
         <v>84</v>
-      </c>
-      <c r="B43" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
         <v>86</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
         <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
         <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
         <v>92</v>
-      </c>
-      <c r="B47" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
         <v>94</v>
-      </c>
-      <c r="B48" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
         <v>96</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" t="s">
         <v>98</v>
-      </c>
-      <c r="B50" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
         <v>100</v>
-      </c>
-      <c r="B51" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
         <v>102</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
         <v>104</v>
-      </c>
-      <c r="B53" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" t="s">
         <v>106</v>
-      </c>
-      <c r="B54" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" t="s">
         <v>108</v>
-      </c>
-      <c r="B55" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" t="s">
         <v>110</v>
-      </c>
-      <c r="B56" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" t="s">
         <v>112</v>
-      </c>
-      <c r="B57" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" t="s">
         <v>114</v>
-      </c>
-      <c r="B58" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" t="s">
         <v>116</v>
-      </c>
-      <c r="B59" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s">
         <v>118</v>
-      </c>
-      <c r="B60" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" t="s">
         <v>120</v>
-      </c>
-      <c r="B61" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B80" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B82" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B84" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B85" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B88" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B89" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B92" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B94" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B96" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B97" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B98" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B103" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B104" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B105" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B106" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B107" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B108" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B109" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B110" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B111" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B113" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B114" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B115" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B116" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B117" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B118" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B119" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B120" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B121" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B122" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B123" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B125" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B126" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B127" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B128" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B129" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B130" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B131" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B132" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B133" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B134" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B135" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B136" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B137" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B138" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B139" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B140" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B141" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B142" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B143" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B144" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B145" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B146" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B147" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B148" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B149" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B150" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B151" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B152" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B153" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B154" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B155" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B156" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B157" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B158" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B159" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B160" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B161" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B162" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B163" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B164" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B165" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B166" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B167" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B168" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B169" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B170" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B171" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B172" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B173" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B174" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B175" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B176" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B177" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B178" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B179" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B180" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B181" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B182" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B183" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B184" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B185" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B186" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B187" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B188" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B189" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B190" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B191" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B192" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B193" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B194" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B195" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B196" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B197" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B198" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B199" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B200" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B201" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B202" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B203" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B204" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B205" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B206" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B207" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B208" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B209" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B210" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B211" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B212" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B213" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B214" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B215" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B216" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B217" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B218" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B219" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B220" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B221" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B222" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B223" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B224" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B225" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B226" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B227" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B228" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B229" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B230" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B231" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B232" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B233" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B234" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B235" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B236" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B237" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B238" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B239" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B240" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B241" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B242" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B243" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B244" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B245" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B246" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B247" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B248" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B249" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B250" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B251" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B252" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B253" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B254" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B255" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B256" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B257" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B258" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B259" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B260" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B261" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B262" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B263" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B264" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B265" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B266" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B267" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B268" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B269" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B270" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B271" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B272" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B273" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B274" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B275" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B276" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B277" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B278" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B279" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B280" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B281" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B282" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B283" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B284" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B285" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B286" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B287" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B288" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B289" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B290" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B291" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B292" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B293" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B294" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B295" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B296" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B297" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B298" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B299" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B300" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B301" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B302" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B303" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B304" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B305" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B306" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B307" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B308" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B309" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B310" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B311" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B312" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B313" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B314" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B315" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B316" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B317" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B318" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B319" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B320" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B321" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B322" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B323" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B324" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B325" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B326" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B327" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B328" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B329" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B330" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B331" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B332" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B333" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B334" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B335" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B336" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B337" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B338" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B339" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>